<commit_message>
Update soer, rumus masih diragukan
</commit_message>
<xml_diff>
--- a/RAB Panel Surya.xlsx
+++ b/RAB Panel Surya.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="13080" activeTab="1"/>
+    <workbookView windowWidth="28125" windowHeight="13080"/>
   </bookViews>
   <sheets>
     <sheet name="RAB" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
     <t>Inverter</t>
   </si>
   <si>
-    <t>https://www.tokopedia.com/gudangpanelsurya/power-inverter-stec-stc-dc-to-ac-100watt-12v-100w-modif-100-w?extParam=ivf%3Dfalse%26src%3Dsearch&amp;refined=true</t>
+    <t xml:space="preserve">https://www.tokopedia.com/gudangpanelsurya/power-inverter-stec-stc-dc-to-ac-100watt-12v-100w-modif-100-w?extParam=ivf%3Dfalse%26src%3Dsearch&amp;refined=true </t>
   </si>
   <si>
     <t>Total</t>
@@ -768,7 +768,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -837,6 +837,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1188,8 +1191,8 @@
   </sheetPr>
   <dimension ref="B1:I15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1296,7 +1299,7 @@
         <f>E6*G6</f>
         <v>65000</v>
       </c>
-      <c r="I6" s="25" t="s">
+      <c r="I6" s="26" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1350,7 +1353,7 @@
         <f>E8*G8</f>
         <v>160000</v>
       </c>
-      <c r="I8" s="20" t="s">
+      <c r="I8" s="27" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1390,8 +1393,9 @@
     <mergeCell ref="B2:I2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="I5" r:id="rId1" display="https://www.tokopedia.com/rr-elektrik/solar-panel-solar-cell-panel-surya-gh-100wp-mono-tanpa-peti?extParam=ivf%3Dfalse%26src%3Dsearch"/>
-    <hyperlink ref="I6" r:id="rId2" display="https://www.tokopedia.com/mediatamait/solar-charge-controller-scc-10a-20a-30a-cell-pwm-12v24v-20-ampere?extParam=ivf%3Dfalse%26src%3Dsearch%26whid%3D9767451"/>
+    <hyperlink ref="I5" r:id="rId1" display="https://www.tokopedia.com/rr-elektrik/solar-panel-solar-cell-panel-surya-gh-100wp-mono-tanpa-peti?extParam=ivf%3Dfalse%26src%3Dsearch" tooltip="https://www.tokopedia.com/rr-elektrik/solar-panel-solar-cell-panel-surya-gh-100wp-mono-tanpa-peti?extParam=ivf%3Dfalse%26src%3Dsearch"/>
+    <hyperlink ref="I8" r:id="rId2" display="https://www.tokopedia.com/gudangpanelsurya/power-inverter-stec-stc-dc-to-ac-100watt-12v-100w-modif-100-w?extParam=ivf%3Dfalse%26src%3Dsearch&amp;refined=true "/>
+    <hyperlink ref="I6" r:id="rId3" display="https://www.tokopedia.com/mediatamait/solar-charge-controller-scc-10a-20a-30a-cell-pwm-12v24v-20-ampere?extParam=ivf%3Dfalse%26src%3Dsearch%26whid%3D9767451"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -1403,7 +1407,7 @@
   <sheetPr/>
   <dimension ref="B2:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>

</xml_diff>